<commit_message>
Analytics code updated Fixed adsense
</commit_message>
<xml_diff>
--- a/Courier_master.xlsx
+++ b/Courier_master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Websites/PHP Storm/PHPstorm/Courier_New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9AD8C1-BD73-5C42-99B0-7DEBAEEC0915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC21D0E1-6D7C-6A44-A0E9-4D92E181457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{CD973A7E-17AB-B142-BBE6-39C3A698DDBF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5010" uniqueCount="3087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5013" uniqueCount="3090">
   <si>
     <t>vendor_id</t>
   </si>
@@ -9299,6 +9299,15 @@
   </si>
   <si>
     <t>https://www.relaxofootwear.com/track-order</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.zeptoconsumerapp</t>
+  </si>
+  <si>
+    <t>Zepto Groceries</t>
+  </si>
+  <si>
+    <t>zeptogroceries</t>
   </si>
 </sst>
 </file>
@@ -9460,7 +9469,27 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -17274,10 +17303,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B434:B437">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B437">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B279" r:id="rId1" display="http://phoenixcpl.com/tracking.asp" xr:uid="{BCF09F8F-BE57-0243-99E6-A0119F8A7FE7}"/>
@@ -22020,10 +22049,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B248">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B249:B252 B2:B247">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D26" r:id="rId1" xr:uid="{B7A49A68-7EB7-2D41-B742-1F7D123B4054}"/>
@@ -22187,10 +22216,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239C2847-50B1-F641-AA1D-D5C5057BE439}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22403,13 +22432,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>699</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3088</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3089</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3087</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="D13">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{A9510FB5-6866-2440-9B19-E6B6758C3B4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>